<commit_message>
Documentation Update : sprint budown charts (1-6), tracking file, usecase description.
</commit_message>
<xml_diff>
--- a/documentation/tracking.xlsx
+++ b/documentation/tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patih\Desktop\Bachelor\bpr2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94102304-FD1A-43FE-8BBE-64913A0F8E1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074B7CF2-3CB1-48AC-83EB-C05F65EE61C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52AF06BC-8BB3-4933-8457-EF3B53D3F408}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{52AF06BC-8BB3-4933-8457-EF3B53D3F408}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Patrik Ihnat</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Project report</t>
+  </si>
+  <si>
+    <t>dokoncit sprint burdowncharts (sprint1-6)</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,8 +90,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,14 +120,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -433,16 +455,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F93BD29-266C-43F8-A982-535EF5B3F6F3}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +479,7 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -485,12 +507,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B87C5725692D194582D384060B21F30E" ma:contentTypeVersion="5" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="d229b8881ff79ff6f21f778ad9c14fe6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c21484e5-d2b2-457e-8d82-4946e0bf2238" xmlns:ns4="5028aaee-70dd-4999-a310-3efcabddf5e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87690ac462d9c9089d0285ef82429d0a" ns3:_="" ns4:_="">
     <xsd:import namespace="c21484e5-d2b2-457e-8d82-4946e0bf2238"/>
@@ -661,7 +694,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -670,13 +703,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9274767-9A18-4089-BE2E-5033D2BB728B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="5028aaee-70dd-4999-a310-3efcabddf5e6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c21484e5-d2b2-457e-8d82-4946e0bf2238"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6038B5-AE9A-4DF4-871B-776A20667049}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -695,27 +739,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{770DD98E-B246-4EBF-8A58-963F3A9BA9A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9274767-9A18-4089-BE2E-5033D2BB728B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5028aaee-70dd-4999-a310-3efcabddf5e6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c21484e5-d2b2-457e-8d82-4946e0bf2238"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Documentation Update : process report, left out tasks in tracking file
</commit_message>
<xml_diff>
--- a/documentation/tracking.xlsx
+++ b/documentation/tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patih\Desktop\Bachelor\bpr2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074B7CF2-3CB1-48AC-83EB-C05F65EE61C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1181D54-D59C-4FB7-BB20-2149F6DA1313}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{52AF06BC-8BB3-4933-8457-EF3B53D3F408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Patrik Ihnat</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>dokoncit sprint burdowncharts (sprint1-6)</t>
+  </si>
+  <si>
+    <t>eer diagram</t>
+  </si>
+  <si>
+    <t>sequence diagram</t>
+  </si>
+  <si>
+    <t>Process report 6-8 sprinty prerobit dokmumentaciu</t>
   </si>
 </sst>
 </file>
@@ -77,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +105,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,17 +135,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -139,8 +143,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -455,16 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F93BD29-266C-43F8-A982-535EF5B3F6F3}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,15 +483,15 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -495,7 +499,7 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -508,8 +512,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>